<commit_message>
hemos agregado nuevos metodos en la clase AddressBook
</commit_message>
<xml_diff>
--- a/Documentos/Formato PSP Arteaga_libreta.xlsx
+++ b/Documentos/Formato PSP Arteaga_libreta.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerli\Desktop\Repositorios\Arteaga_libreta-de-direcciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerli\Desktop\Repositorios\Arteaga_libreta-de-direcciones\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D44127-C77D-43F0-8435-05EA3A87BD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0742988D-76EE-433B-B940-E8237EA5C7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="3" activeTab="6" xr2:uid="{5C91324D-6205-4AF6-A214-4DE2B566EAE9}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="136">
   <si>
     <t>ESTANDARES DE CODIFICACIÓN</t>
   </si>
@@ -507,6 +507,36 @@
   </si>
   <si>
     <t>Gerly Daniel Arteaga Bernal</t>
+  </si>
+  <si>
+    <t>diseño</t>
+  </si>
+  <si>
+    <t>interrupcion causada por responder mensajes</t>
+  </si>
+  <si>
+    <t>desarrollo</t>
+  </si>
+  <si>
+    <t>Interrupcion causada por ingerir alimentos</t>
+  </si>
+  <si>
+    <t>20 minutos</t>
+  </si>
+  <si>
+    <t>Error al generar una clase "Lista" cuando no era necesaria</t>
+  </si>
+  <si>
+    <t>Sin comentarios</t>
+  </si>
+  <si>
+    <t>Desarrollo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 minutos </t>
+  </si>
+  <si>
+    <t>error en un do while</t>
   </si>
 </sst>
 </file>
@@ -757,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -819,8 +849,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -840,19 +889,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -867,8 +904,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -880,12 +932,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -912,18 +958,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -934,9 +968,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -945,10 +976,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1417,180 +1451,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" ht="55.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="35" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8" ht="201.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="32" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="32" t="s">
+      <c r="B5" s="28"/>
+      <c r="C5" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:8" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="32" t="s">
+      <c r="B6" s="28"/>
+      <c r="C6" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
     </row>
     <row r="7" spans="1:8" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="28"/>
+      <c r="C7" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="29" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
     </row>
     <row r="9" spans="1:8" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="26" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:8" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="26" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="35"/>
     </row>
     <row r="11" spans="1:8" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26" t="s">
+      <c r="B11" s="28"/>
+      <c r="C11" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:8" ht="150.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26" t="s">
+      <c r="B12" s="28"/>
+      <c r="C12" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -1602,6 +1626,16 @@
     <mergeCell ref="C11:H11"/>
     <mergeCell ref="C12:H12"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1622,107 +1656,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="1:9" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36" t="s">
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:9" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36" t="s">
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
     </row>
     <row r="5" spans="1:9" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="36" t="s">
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36" t="s">
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
     </row>
     <row r="6" spans="1:9" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="36" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36" t="s">
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="D3:F3"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="G6:I6"/>
@@ -1732,6 +1761,11 @@
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1754,16 +1788,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -1787,20 +1821,20 @@
       <c r="AC1" s="5"/>
     </row>
     <row r="2" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
       <c r="D2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -1824,14 +1858,14 @@
       <c r="AC2" s="5"/>
     </row>
     <row r="3" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1855,20 +1889,20 @@
       <c r="AC3" s="5"/>
     </row>
     <row r="4" spans="1:29" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="44"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="50"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="56"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -1892,18 +1926,18 @@
       <c r="AC4" s="5"/>
     </row>
     <row r="5" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="47"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -1927,18 +1961,18 @@
       <c r="AC5" s="5"/>
     </row>
     <row r="6" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="47"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="56"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="58"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -1963,17 +1997,17 @@
     </row>
     <row r="7" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="47"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -1998,17 +2032,17 @@
     </row>
     <row r="8" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="47"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -2033,17 +2067,17 @@
     </row>
     <row r="9" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="47"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -2068,17 +2102,17 @@
     </row>
     <row r="10" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -2102,18 +2136,18 @@
       <c r="AC10" s="5"/>
     </row>
     <row r="11" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="53"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="56"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="58"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="49"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -2138,17 +2172,17 @@
     </row>
     <row r="12" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="55"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -4799,16 +4833,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:C3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="B8:C8"/>
     <mergeCell ref="E12:H12"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
@@ -4821,6 +4845,16 @@
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:C3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4844,22 +4878,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="61"/>
+      <c r="C5" s="63"/>
       <c r="D5" s="19" t="s">
         <v>59</v>
       </c>
@@ -4871,10 +4905,10 @@
       <c r="A6" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="63" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="61"/>
+      <c r="C6" s="63"/>
       <c r="D6" s="19" t="s">
         <v>93</v>
       </c>
@@ -5119,8 +5153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B58D6D67-2B34-4A51-9CD1-D434E752461B}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5141,15 +5175,15 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:7" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -5175,33 +5209,76 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="67">
+      <c r="A6" s="25">
         <v>45434</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="69">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C6" s="69">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D6" s="69">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E6" s="69">
+        <f>(C6-B6)-D6</f>
+        <v>1.3888888888888892E-2</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="A7" s="25">
+        <v>45435</v>
+      </c>
+      <c r="B7" s="69">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C7" s="69">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="69">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E7" s="69">
+        <f>(C7-B7)-D7</f>
+        <v>3.8194444444444482E-2</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="A8" s="25">
+        <v>45437</v>
+      </c>
+      <c r="B8" s="69">
+        <v>0.92361111111111116</v>
+      </c>
+      <c r="C8" s="69">
+        <v>0.9770833333333333</v>
+      </c>
+      <c r="D8" s="69">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="E8" s="69">
+        <f>(C8-B8)-D8</f>
+        <v>5.2777777777777701E-2</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
@@ -5245,7 +5322,7 @@
   <dimension ref="A3:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5261,197 +5338,197 @@
   <sheetData>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:7" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66" t="s">
+      <c r="C6" s="67"/>
+      <c r="D6" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>10</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="63" t="s">
+      <c r="C7" s="65"/>
+      <c r="D7" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>20</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="63" t="s">
+      <c r="C8" s="65"/>
+      <c r="D8" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>30</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="63" t="s">
+      <c r="C9" s="65"/>
+      <c r="D9" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>40</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="63" t="s">
+      <c r="C10" s="65"/>
+      <c r="D10" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>50</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="63" t="s">
+      <c r="C11" s="65"/>
+      <c r="D11" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>60</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="63" t="s">
+      <c r="C12" s="65"/>
+      <c r="D12" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>70</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="64"/>
-      <c r="D13" s="63" t="s">
+      <c r="C13" s="65"/>
+      <c r="D13" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>80</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="64"/>
-      <c r="D14" s="63" t="s">
+      <c r="C14" s="65"/>
+      <c r="D14" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>90</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="63" t="s">
+      <c r="C15" s="65"/>
+      <c r="D15" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>10</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="64"/>
-      <c r="D16" s="63" t="s">
+      <c r="C16" s="65"/>
+      <c r="D16" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
       <c r="F18" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="68">
+      <c r="G18" s="26">
         <v>45434</v>
       </c>
     </row>
@@ -5482,27 +5559,41 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
+      <c r="A21" s="70">
+        <v>45435</v>
+      </c>
       <c r="B21" s="3">
         <v>1</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="C21" s="3">
+        <v>30</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
+      <c r="B23" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63"/>
     </row>
     <row r="25" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
@@ -5528,27 +5619,41 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
+      <c r="A26" s="70">
+        <v>45802</v>
+      </c>
       <c r="B26" s="3">
         <v>2</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="C26" s="3">
+        <v>20</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
+      <c r="B28" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="63"/>
     </row>
     <row r="30" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
@@ -5589,12 +5694,12 @@
       <c r="A33" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
     </row>
     <row r="34" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
@@ -5635,12 +5740,12 @@
       <c r="A37" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="61"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="61"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="63"/>
     </row>
     <row r="38" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
@@ -5681,25 +5786,33 @@
       <c r="A41" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B41" s="61"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:G7"/>
     <mergeCell ref="B41:G41"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:G7"/>
     <mergeCell ref="D8:G8"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="D14:G14"/>
@@ -5711,29 +5824,13 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007C3FE6271BEA2C45BD053C062D34DAB8" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="8c4fe01e16a7d30497b436951f273215">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="302a697f-c05b-4e64-9398-25fe8623ee8c" xmlns:ns4="0f6e5129-90bf-4ef3-b1b4-c0d43a9656e6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="00a4e6a6de0be021f3e45b28a1c15569" ns3:_="" ns4:_="">
     <xsd:import namespace="302a697f-c05b-4e64-9398-25fe8623ee8c"/>
@@ -5986,6 +6083,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5995,14 +6101,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2504083-5C3D-4649-9EFF-1D07A6C3996D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E14591D-47D5-498B-B18C-CA60E582947C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6017,6 +6115,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2504083-5C3D-4649-9EFF-1D07A6C3996D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
we update the psp format
</commit_message>
<xml_diff>
--- a/Documentos/Formato PSP Arteaga_libreta.xlsx
+++ b/Documentos/Formato PSP Arteaga_libreta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerli\Desktop\Repositorios\Arteaga_libreta-de-direcciones\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerli\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0742988D-76EE-433B-B940-E8237EA5C7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8BBFF7-1748-44B6-AD52-4FB3BEE82CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="3" activeTab="6" xr2:uid="{5C91324D-6205-4AF6-A214-4DE2B566EAE9}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="154">
   <si>
     <t>ESTANDARES DE CODIFICACIÓN</t>
   </si>
@@ -446,12 +446,6 @@
     <t>A la fecha%</t>
   </si>
   <si>
-    <t xml:space="preserve">Total real </t>
-  </si>
-  <si>
-    <t>Estimado (planeado)</t>
-  </si>
-  <si>
     <t>Real</t>
   </si>
   <si>
@@ -465,16 +459,10 @@
     <t>NO</t>
   </si>
   <si>
-    <t>Total real + actual</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cuántos fueron </t>
   </si>
   <si>
     <t>Total real (cuántos fueron)+ actual</t>
-  </si>
-  <si>
-    <t>%Total real + actual</t>
   </si>
   <si>
     <t>Total real (cuántos fueron+real)</t>
@@ -500,9 +488,6 @@
     <t xml:space="preserve">Jose Antonio Vergara Camacho </t>
   </si>
   <si>
-    <t>22 de mayo de 2024</t>
-  </si>
-  <si>
     <t>Java</t>
   </si>
   <si>
@@ -537,6 +522,75 @@
   </si>
   <si>
     <t>error en un do while</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminada la parte de desarrollo </t>
+  </si>
+  <si>
+    <t>Terminado el diagrama de clases</t>
+  </si>
+  <si>
+    <t>Revisando excepciones lanzadas por desborde de memoria</t>
+  </si>
+  <si>
+    <t>15 minutos</t>
+  </si>
+  <si>
+    <t>Error de version del junit (dependencia de pruebas)</t>
+  </si>
+  <si>
+    <t>Referencia incorrecta hacia una lista no declarada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68 minutos </t>
+  </si>
+  <si>
+    <t>68  minutos</t>
+  </si>
+  <si>
+    <t>60 minutos</t>
+  </si>
+  <si>
+    <t>300 minutos</t>
+  </si>
+  <si>
+    <t>293 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40 minutos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 minutos </t>
+  </si>
+  <si>
+    <t>5 minutos</t>
+  </si>
+  <si>
+    <t>07 de junio de 2024</t>
+  </si>
+  <si>
+    <t>25 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">420 minutos </t>
+  </si>
+  <si>
+    <t>391  minutos</t>
+  </si>
+  <si>
+    <t>391 minutos</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>150 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60 minutos </t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -606,15 +660,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -783,11 +843,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -853,6 +924,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -970,19 +1045,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1451,166 +1535,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" spans="1:8" ht="55.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" ht="201.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="1:8" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="31" t="s">
+      <c r="B5" s="30"/>
+      <c r="C5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="33" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="35"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="36" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="40"/>
     </row>
     <row r="9" spans="1:8" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="35"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="1:8" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="33" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="35"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="33" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" ht="150.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="33" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="35"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1656,98 +1740,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30" t="s">
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
     </row>
     <row r="4" spans="1:9" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30" t="s">
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
     </row>
     <row r="5" spans="1:9" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="30" t="s">
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30" t="s">
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
     </row>
     <row r="6" spans="1:9" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="30" t="s">
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30" t="s">
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1788,16 +1872,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -1821,20 +1905,20 @@
       <c r="AC1" s="5"/>
     </row>
     <row r="2" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -1858,14 +1942,14 @@
       <c r="AC2" s="5"/>
     </row>
     <row r="3" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1889,20 +1973,20 @@
       <c r="AC3" s="5"/>
     </row>
     <row r="4" spans="1:29" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="56"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="58"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -1926,18 +2010,18 @@
       <c r="AC4" s="5"/>
     </row>
     <row r="5" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -1961,18 +2045,18 @@
       <c r="AC5" s="5"/>
     </row>
     <row r="6" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="46"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="47"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -1997,17 +2081,17 @@
     </row>
     <row r="7" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -2032,17 +2116,17 @@
     </row>
     <row r="8" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -2067,17 +2151,17 @@
     </row>
     <row r="9" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -2102,17 +2186,17 @@
     </row>
     <row r="10" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -2136,18 +2220,18 @@
       <c r="AC10" s="5"/>
     </row>
     <row r="11" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="58"/>
-      <c r="C11" s="59"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="47"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="51"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -2172,17 +2256,17 @@
     </row>
     <row r="12" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="61"/>
+      <c r="C12" s="63"/>
       <c r="D12" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -4862,10 +4946,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35175C74-1589-4401-92EC-A60D5C8F9D38}">
-  <dimension ref="A3:E31"/>
+  <dimension ref="A3:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4877,46 +4961,46 @@
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="62" t="s">
+    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="63" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="63"/>
+      <c r="B5" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="65"/>
       <c r="D5" s="19" t="s">
         <v>59</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="63" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" s="63"/>
+      <c r="B6" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="65"/>
       <c r="D6" s="19" t="s">
         <v>93</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>94</v>
       </c>
@@ -4924,7 +5008,7 @@
         <v>46</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>47</v>
@@ -4933,73 +5017,131 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>151</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="E9" s="20">
+        <v>40</v>
+      </c>
+      <c r="F9" s="73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="22">
+        <v>113.33</v>
+      </c>
+      <c r="F10" s="73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="20"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11" s="20">
+        <v>97.67</v>
+      </c>
+      <c r="F11" s="73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="22">
+        <v>125</v>
+      </c>
+      <c r="F12" s="73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="22">
+        <v>12.5</v>
+      </c>
+      <c r="F13" s="73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="22"/>
+      <c r="B14" s="78" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="78" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="79" t="s">
+        <v>149</v>
+      </c>
       <c r="E14" s="22"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="73"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>47</v>
@@ -5013,22 +5155,25 @@
         <v>95</v>
       </c>
       <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>114</v>
-      </c>
       <c r="E17" s="20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
+      <c r="B18" t="s">
+        <v>109</v>
+      </c>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -5037,32 +5182,66 @@
       <c r="A19" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="20"/>
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="C19" s="22">
+        <v>5</v>
+      </c>
+      <c r="D19" s="22">
+        <v>5</v>
+      </c>
+      <c r="E19" s="74">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20" s="22">
+        <v>50</v>
+      </c>
+      <c r="D20" s="22">
+        <v>50</v>
+      </c>
+      <c r="E20" s="75">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>99</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" s="22">
+        <v>8</v>
+      </c>
+      <c r="D21" s="22">
+        <v>8</v>
+      </c>
+      <c r="E21" s="76">
+        <v>0.626</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="22"/>
+      <c r="B22" s="77">
+        <v>30</v>
+      </c>
+      <c r="C22" s="78">
+        <v>63</v>
+      </c>
+      <c r="D22" s="79">
+        <v>63</v>
+      </c>
       <c r="E22" s="22"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -5073,7 +5252,7 @@
         <v>46</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D24" s="21" t="s">
         <v>47</v>
@@ -5086,6 +5265,9 @@
       <c r="A25" t="s">
         <v>102</v>
       </c>
+      <c r="B25" t="s">
+        <v>153</v>
+      </c>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
@@ -5094,6 +5276,9 @@
       <c r="A26" t="s">
         <v>48</v>
       </c>
+      <c r="B26" t="s">
+        <v>153</v>
+      </c>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
@@ -5102,32 +5287,66 @@
       <c r="A27" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="20"/>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" s="22">
+        <v>5</v>
+      </c>
+      <c r="D27" s="22">
+        <v>5</v>
+      </c>
+      <c r="E27" s="74">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
+      <c r="B28">
+        <v>50</v>
+      </c>
+      <c r="C28" s="22">
+        <v>50</v>
+      </c>
+      <c r="D28" s="22">
+        <v>50</v>
+      </c>
+      <c r="E28" s="74">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29" s="22">
+        <v>8</v>
+      </c>
+      <c r="D29" s="22">
+        <v>8</v>
+      </c>
+      <c r="E29" s="74">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="22"/>
+      <c r="B30" s="77">
+        <v>63</v>
+      </c>
+      <c r="C30" s="78">
+        <v>63</v>
+      </c>
+      <c r="D30" s="79">
+        <v>63</v>
+      </c>
       <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -5154,7 +5373,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5170,20 +5389,20 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:7" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -5199,7 +5418,7 @@
         <v>54</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>55</v>
@@ -5212,102 +5431,138 @@
       <c r="A6" s="25">
         <v>45434</v>
       </c>
-      <c r="B6" s="69">
+      <c r="B6" s="27">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C6" s="69">
+      <c r="C6" s="27">
         <v>3.125E-2</v>
       </c>
-      <c r="D6" s="69">
+      <c r="D6" s="27">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="E6" s="69">
+      <c r="E6" s="27">
         <f>(C6-B6)-D6</f>
         <v>1.3888888888888892E-2</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25">
         <v>45435</v>
       </c>
-      <c r="B7" s="69">
+      <c r="B7" s="27">
         <v>0.69791666666666663</v>
       </c>
-      <c r="C7" s="69">
+      <c r="C7" s="27">
         <v>0.75</v>
       </c>
-      <c r="D7" s="69">
+      <c r="D7" s="27">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="E7" s="69">
+      <c r="E7" s="27">
         <f>(C7-B7)-D7</f>
         <v>3.8194444444444482E-2</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>128</v>
+      <c r="F7" s="72" t="s">
+        <v>123</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25">
         <v>45437</v>
       </c>
-      <c r="B8" s="69">
+      <c r="B8" s="27">
         <v>0.92361111111111116</v>
       </c>
-      <c r="C8" s="69">
+      <c r="C8" s="27">
         <v>0.9770833333333333</v>
       </c>
-      <c r="D8" s="69">
+      <c r="D8" s="27">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="E8" s="69">
+      <c r="E8" s="27">
         <f>(C8-B8)-D8</f>
         <v>5.2777777777777701E-2</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>128</v>
+      <c r="F8" s="72" t="s">
+        <v>123</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
+        <v>45450</v>
+      </c>
+      <c r="B9" s="27">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="C9" s="27">
+        <v>0.38124999999999998</v>
+      </c>
+      <c r="D9" s="27">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="E9" s="27">
+        <f>(C9-B9)-D9</f>
+        <v>7.9166666666666649E-2</v>
+      </c>
+      <c r="F9" s="72" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <v>45450</v>
+      </c>
+      <c r="B10" s="27">
+        <v>0.38263888888888886</v>
+      </c>
+      <c r="C10" s="27">
+        <v>0.41597222222222224</v>
+      </c>
+      <c r="D10" s="27">
+        <v>0</v>
+      </c>
+      <c r="E10" s="27">
+        <f>(C10-B10)-D10</f>
+        <v>3.3333333333333381E-2</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
     <row r="11" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="25">
+        <v>45450</v>
+      </c>
+      <c r="B11" s="27">
+        <v>0.41319444444444442</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="71"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:G4"/>
@@ -5321,8 +5576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1E9371-A978-4959-97B1-907507EF065D}">
   <dimension ref="A3:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5338,40 +5593,40 @@
   <sheetData>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:7" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67" t="s">
+      <c r="C6" s="70"/>
+      <c r="D6" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>10</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="65"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="68" t="s">
         <v>71</v>
       </c>
@@ -5383,10 +5638,10 @@
       <c r="A8" s="2">
         <v>20</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="65"/>
+      <c r="C8" s="67"/>
       <c r="D8" s="68" t="s">
         <v>72</v>
       </c>
@@ -5398,10 +5653,10 @@
       <c r="A9" s="2">
         <v>30</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="65"/>
+      <c r="C9" s="67"/>
       <c r="D9" s="68" t="s">
         <v>73</v>
       </c>
@@ -5413,10 +5668,10 @@
       <c r="A10" s="2">
         <v>40</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="65"/>
+      <c r="C10" s="67"/>
       <c r="D10" s="68" t="s">
         <v>74</v>
       </c>
@@ -5428,10 +5683,10 @@
       <c r="A11" s="2">
         <v>50</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="65"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="68" t="s">
         <v>75</v>
       </c>
@@ -5443,10 +5698,10 @@
       <c r="A12" s="2">
         <v>60</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="65"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="68" t="s">
         <v>76</v>
       </c>
@@ -5458,10 +5713,10 @@
       <c r="A13" s="2">
         <v>70</v>
       </c>
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="65"/>
+      <c r="C13" s="67"/>
       <c r="D13" s="68" t="s">
         <v>77</v>
       </c>
@@ -5473,10 +5728,10 @@
       <c r="A14" s="2">
         <v>80</v>
       </c>
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="65"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="68" t="s">
         <v>78</v>
       </c>
@@ -5488,10 +5743,10 @@
       <c r="A15" s="2">
         <v>90</v>
       </c>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="65"/>
+      <c r="C15" s="67"/>
       <c r="D15" s="68" t="s">
         <v>79</v>
       </c>
@@ -5503,10 +5758,10 @@
       <c r="A16" s="2">
         <v>10</v>
       </c>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="65"/>
+      <c r="C16" s="67"/>
       <c r="D16" s="68" t="s">
         <v>80</v>
       </c>
@@ -5519,12 +5774,12 @@
       <c r="A18" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="63" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
+      <c r="B18" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
       <c r="F18" s="10" t="s">
         <v>59</v>
       </c>
@@ -5546,10 +5801,10 @@
         <v>89</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>81</v>
@@ -5559,7 +5814,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="70">
+      <c r="A21" s="28">
         <v>45435</v>
       </c>
       <c r="B21" s="3">
@@ -5569,13 +5824,13 @@
         <v>30</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G21" s="3">
         <v>1</v>
@@ -5586,14 +5841,14 @@
       <c r="A23" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="63" t="s">
-        <v>131</v>
-      </c>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
+      <c r="B23" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
     </row>
     <row r="25" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
@@ -5606,7 +5861,7 @@
         <v>89</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>90</v>
@@ -5619,7 +5874,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="70">
+      <c r="A26" s="28">
         <v>45802</v>
       </c>
       <c r="B26" s="3">
@@ -5629,13 +5884,13 @@
         <v>20</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G26" s="3">
         <v>1</v>
@@ -5646,14 +5901,14 @@
       <c r="A28" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="63" t="s">
-        <v>135</v>
-      </c>
-      <c r="C28" s="63"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="63"/>
+      <c r="B28" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
     </row>
     <row r="30" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
@@ -5666,7 +5921,7 @@
         <v>89</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>90</v>
@@ -5679,27 +5934,41 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
+      <c r="A31" s="28">
+        <v>45450</v>
+      </c>
       <c r="B31" s="3">
         <v>3</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="C31" s="3">
+        <v>60</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
+      <c r="B33" s="65" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
     </row>
     <row r="34" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
@@ -5712,7 +5981,7 @@
         <v>89</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>90</v>
@@ -5725,27 +5994,41 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
+      <c r="A35" s="28">
+        <v>45450</v>
+      </c>
       <c r="B35" s="3">
         <v>4</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
+      <c r="C35" s="3">
+        <v>10</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="63"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
+      <c r="B37" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="65"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
     </row>
     <row r="38" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
@@ -5758,7 +6041,7 @@
         <v>89</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>90</v>
@@ -5771,27 +6054,41 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
+      <c r="A39" s="28">
+        <v>45450</v>
+      </c>
       <c r="B39" s="3">
         <v>5</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
+      <c r="C39" s="3">
+        <v>80</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G39" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B41" s="63"/>
-      <c r="C41" s="63"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="63"/>
+      <c r="B41" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" s="65"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="65"/>
+      <c r="G41" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="29">

</xml_diff>